<commit_message>
Final changes still Eng,Common,Utils
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017889_CommentsAndContactsMappingToEngUponConversionFromOpportunity.xlsx
+++ b/TestData/TMTT0017889_CommentsAndContactsMappingToEngUponConversionFromOpportunity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGoyal0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01835E44-CBEF-436F-B4B0-CF57B62887CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A452D6EB-6F55-4E50-A6ED-C9E838B619C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
   <si>
     <t>Client</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>Buyside</t>
-  </si>
-  <si>
-    <t>Rob Oudman</t>
   </si>
   <si>
     <t>Michael Birney</t>
@@ -602,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,10 +734,10 @@
         <v>65</v>
       </c>
       <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
         <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>79</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -767,7 +764,7 @@
         <v>16</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>35</v>
@@ -785,7 +782,7 @@
         <v>24</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U2" t="s">
         <v>27</v>
@@ -845,13 +842,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -877,26 +874,26 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>